<commit_message>
After adding switch for the calculation of BKG/OFFSET/INTERCEPT
</commit_message>
<xml_diff>
--- a/result files/Instrument Working Zone.xlsx
+++ b/result files/Instrument Working Zone.xlsx
@@ -8,29 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://biocartis-my.sharepoint.com/personal/eshahraeeni_biocartis_com/Documents/Documents/Python/INS Characterization/Python/result files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="11_5B9174A087C0574DBFFA3211595ED87656CDFCB1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7C6EF709-1197-4AAD-B3D2-C5D866794233}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="11_4185F6A28760D173AF9B2C11595ED87656CDE376" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ABAA172F-BC5F-4A3D-A635-65C8C02279F5}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3510" yWindow="3510" windowWidth="38700" windowHeight="15555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$73</definedName>
-  </definedNames>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -446,19 +431,10 @@
   <dimension ref="A1:H73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -500,16 +476,16 @@
         <v>1</v>
       </c>
       <c r="E2">
-        <v>86.700808537321478</v>
+        <v>86.700808537321521</v>
       </c>
       <c r="F2">
-        <v>5.0556147999999999</v>
+        <v>4.4788177337142798</v>
       </c>
       <c r="G2">
         <v>2.6287683999999998</v>
       </c>
       <c r="H2">
-        <v>3.4233554464723701</v>
+        <v>3.00334350670615</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -526,16 +502,16 @@
         <v>1</v>
       </c>
       <c r="E3">
-        <v>120.1575413736763</v>
+        <v>120.15754137367639</v>
       </c>
       <c r="F3">
-        <v>7.4557979999999997</v>
+        <v>6.5166458494617672</v>
       </c>
       <c r="G3">
         <v>3.8516279999999989</v>
       </c>
       <c r="H3">
-        <v>3.5156829537609271</v>
+        <v>2.4728448246615682</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -552,16 +528,16 @@
         <v>1</v>
       </c>
       <c r="E4">
-        <v>110.186358842193</v>
+        <v>110.1863588421929</v>
       </c>
       <c r="F4">
-        <v>6.2049415999999997</v>
+        <v>5.3824190538817902</v>
       </c>
       <c r="G4">
         <v>2.5268467999999999</v>
       </c>
       <c r="H4">
-        <v>3.4156602316931242</v>
+        <v>3.047558946051661</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -581,13 +557,13 @@
         <v>114.49671178178779</v>
       </c>
       <c r="F5">
-        <v>6.1239052000000003</v>
+        <v>5.3131739319213764</v>
       </c>
       <c r="G5">
         <v>2.6187551999999998</v>
       </c>
       <c r="H5">
-        <v>3.4225994367096928</v>
+        <v>3.0076874145456509</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -604,16 +580,16 @@
         <v>1</v>
       </c>
       <c r="E6">
-        <v>92.684744398684799</v>
+        <v>92.684744398684714</v>
       </c>
       <c r="F6">
-        <v>6.4764624</v>
+        <v>6.0316870093877526</v>
       </c>
       <c r="G6">
         <v>2.8530419999999999</v>
       </c>
       <c r="H6">
-        <v>3.440288398087282</v>
+        <v>2.9060495498059522</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -633,13 +609,13 @@
         <v>101.7289521078588</v>
       </c>
       <c r="F7">
-        <v>7.3611000000000004</v>
+        <v>6.6126621943294239</v>
       </c>
       <c r="G7">
         <v>3.9146744</v>
       </c>
       <c r="H7">
-        <v>3.520443039837462</v>
+        <v>2.4454941524276861</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -656,16 +632,16 @@
         <v>1</v>
       </c>
       <c r="E8">
-        <v>111.382225593594</v>
+        <v>111.3822255935939</v>
       </c>
       <c r="F8">
-        <v>8.0254143999999989</v>
+        <v>7.2667362892438732</v>
       </c>
       <c r="G8">
         <v>4.4187984</v>
       </c>
       <c r="H8">
-        <v>3.5585050645247911</v>
+        <v>2.2267960144018311</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -682,16 +658,16 @@
         <v>1</v>
       </c>
       <c r="E9">
-        <v>91.341999533550862</v>
+        <v>91.341999533550847</v>
       </c>
       <c r="F9">
-        <v>6.0618804000000006</v>
+        <v>5.4328036655628971</v>
       </c>
       <c r="G9">
         <v>2.8195608000000001</v>
       </c>
       <c r="H9">
-        <v>3.43776052347516</v>
+        <v>2.9205743018488439</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -708,16 +684,16 @@
         <v>1</v>
       </c>
       <c r="E10">
-        <v>90.656154224262707</v>
+        <v>90.656154224262679</v>
       </c>
       <c r="F10">
-        <v>6.001188</v>
+        <v>5.3649333177413183</v>
       </c>
       <c r="G10">
         <v>2.4148187999999999</v>
       </c>
       <c r="H10">
-        <v>3.4072019704286891</v>
+        <v>3.096158725087693</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -734,16 +710,16 @@
         <v>1</v>
       </c>
       <c r="E11">
-        <v>82.040544385683788</v>
+        <v>82.040544385683759</v>
       </c>
       <c r="F11">
-        <v>5.5772279999999999</v>
+        <v>4.966786367041049</v>
       </c>
       <c r="G11">
         <v>2.1742544000000001</v>
       </c>
       <c r="H11">
-        <v>3.3890390419989922</v>
+        <v>3.200519926608167</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -760,16 +736,16 @@
         <v>1</v>
       </c>
       <c r="E12">
-        <v>112.3487456636211</v>
+        <v>112.348745663621</v>
       </c>
       <c r="F12">
-        <v>6.4407620000000012</v>
+        <v>5.6531365391350761</v>
       </c>
       <c r="G12">
         <v>2.5511940000000002</v>
       </c>
       <c r="H12">
-        <v>3.4174984772983068</v>
+        <v>3.036996688936064</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -786,16 +762,16 @@
         <v>1</v>
       </c>
       <c r="E13">
-        <v>88.232711370486754</v>
+        <v>88.232711370486726</v>
       </c>
       <c r="F13">
-        <v>5.8884224000000014</v>
+        <v>5.2985347457309624</v>
       </c>
       <c r="G13">
         <v>2.5359908</v>
       </c>
       <c r="H13">
-        <v>3.4163506157132089</v>
+        <v>3.043592112942926</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -815,13 +791,13 @@
         <v>115.58287889446279</v>
       </c>
       <c r="F14">
-        <v>3.5573291999999999</v>
+        <v>2.3985683297230049</v>
       </c>
       <c r="G14">
         <v>2.9277107999999998</v>
       </c>
       <c r="H14">
-        <v>0.53052787683868408</v>
+        <v>0.50915383979438111</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -838,16 +814,16 @@
         <v>2</v>
       </c>
       <c r="E15">
-        <v>170.34555700519601</v>
+        <v>170.34555700519579</v>
       </c>
       <c r="F15">
-        <v>5.5890088000000002</v>
+        <v>3.9782818505757831</v>
       </c>
       <c r="G15">
         <v>4.9014179999999996</v>
       </c>
       <c r="H15">
-        <v>1.005361137077702</v>
+        <v>0.83101414601640133</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -864,16 +840,16 @@
         <v>2</v>
       </c>
       <c r="E16">
-        <v>130.97548096186171</v>
+        <v>130.97548096186159</v>
       </c>
       <c r="F16">
-        <v>3.389543600000001</v>
+        <v>2.1704696332673561</v>
       </c>
       <c r="G16">
         <v>2.9664456000000001</v>
       </c>
       <c r="H16">
-        <v>0.53984667112017926</v>
+        <v>0.51547047814349822</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -890,16 +866,16 @@
         <v>2</v>
       </c>
       <c r="E17">
-        <v>152.6130542265409</v>
+        <v>152.6130542265407</v>
       </c>
       <c r="F17">
-        <v>5.89778</v>
+        <v>4.4389627778190066</v>
       </c>
       <c r="G17">
         <v>5.1054691999999999</v>
       </c>
       <c r="H17">
-        <v>1.054451648857607</v>
+        <v>0.86428958916063792</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -916,16 +892,16 @@
         <v>2</v>
       </c>
       <c r="E18">
-        <v>153.04050167929779</v>
+        <v>153.04050167929759</v>
       </c>
       <c r="F18">
-        <v>5.2805799999999996</v>
+        <v>3.7193576460675</v>
       </c>
       <c r="G18">
         <v>4.2548608000000003</v>
       </c>
       <c r="H18">
-        <v>0.8498128048797895</v>
+        <v>0.72557748429573099</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -942,16 +918,16 @@
         <v>2</v>
       </c>
       <c r="E19">
-        <v>138.389842801144</v>
+        <v>138.38984280114391</v>
       </c>
       <c r="F19">
-        <v>5.2015631999999998</v>
+        <v>3.578928632887493</v>
       </c>
       <c r="G19">
         <v>4.4543903999999994</v>
       </c>
       <c r="H19">
-        <v>0.89781551292188766</v>
+        <v>0.75811557209130509</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -968,16 +944,16 @@
         <v>2</v>
       </c>
       <c r="E20">
-        <v>150.22115351542581</v>
+        <v>150.2211535154259</v>
       </c>
       <c r="F20">
-        <v>7.5380784000000007</v>
+        <v>5.7313223608653594</v>
       </c>
       <c r="G20">
         <v>6.4382320000000011</v>
       </c>
       <c r="H20">
-        <v>1.3750869008591611</v>
+        <v>1.081628535347448</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -994,16 +970,16 @@
         <v>2</v>
       </c>
       <c r="E21">
-        <v>151.03191400849019</v>
+        <v>151.03191400849011</v>
       </c>
       <c r="F21">
-        <v>7.1553495999999992</v>
+        <v>5.7394614186365764</v>
       </c>
       <c r="G21">
         <v>5.6742096000000002</v>
       </c>
       <c r="H21">
-        <v>1.1912788633307789</v>
+        <v>0.95703635489409322</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -1023,13 +999,13 @@
         <v>103.71504866446961</v>
       </c>
       <c r="F22">
-        <v>2.7200443999999999</v>
+        <v>1.9752049242547081</v>
       </c>
       <c r="G22">
         <v>2.2396815999999999</v>
       </c>
       <c r="H22">
-        <v>0.36500223647235058</v>
+        <v>0.39695417360190222</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -1049,13 +1025,13 @@
         <v>125.2784872320818</v>
       </c>
       <c r="F23">
-        <v>6.0944491999999997</v>
+        <v>4.9164980482818814</v>
       </c>
       <c r="G23">
         <v>5.0334595999999996</v>
       </c>
       <c r="H23">
-        <v>1.0371276237253551</v>
+        <v>0.85254669644234315</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -1075,13 +1051,13 @@
         <v>165.20599348704971</v>
       </c>
       <c r="F24">
-        <v>8.1270151999999989</v>
+        <v>6.4902803618680807</v>
       </c>
       <c r="G24">
         <v>6.3942728000000004</v>
       </c>
       <c r="H24">
-        <v>1.364511223649544</v>
+        <v>1.0744599332501981</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -1101,13 +1077,13 @@
         <v>129.33496663943251</v>
       </c>
       <c r="F25">
-        <v>6.518544799999999</v>
+        <v>5.3045885447395662</v>
       </c>
       <c r="G25">
         <v>5.3540568000000004</v>
       </c>
       <c r="H25">
-        <v>1.114256700266951</v>
+        <v>0.9048277607085744</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -1124,16 +1100,16 @@
         <v>3</v>
       </c>
       <c r="E26">
-        <v>56.420887187116037</v>
+        <v>56.420887187116072</v>
       </c>
       <c r="F26">
-        <v>2.2229112</v>
+        <v>0.42689150269222859</v>
       </c>
       <c r="G26">
         <v>1.8023932</v>
       </c>
       <c r="H26">
-        <v>0.44653960393419218</v>
+        <v>0.40744763014106261</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -1150,16 +1126,16 @@
         <v>3</v>
       </c>
       <c r="E27">
-        <v>84.555844730356654</v>
+        <v>84.555844730356611</v>
       </c>
       <c r="F27">
-        <v>3.7199244</v>
+        <v>2.1485621520104701</v>
       </c>
       <c r="G27">
         <v>3.3094839999999999</v>
       </c>
       <c r="H27">
-        <v>0.46194428400444432</v>
+        <v>0.43210375468923612</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -1176,16 +1152,16 @@
         <v>3</v>
       </c>
       <c r="E28">
-        <v>64.624440431030891</v>
+        <v>64.624440431030862</v>
       </c>
       <c r="F28">
-        <v>3.3095028000000002</v>
+        <v>2.0232806735278039</v>
       </c>
       <c r="G28">
         <v>2.9565256</v>
       </c>
       <c r="H28">
-        <v>0.45833653108729561</v>
+        <v>0.42632932738152268</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -1202,16 +1178,16 @@
         <v>3</v>
       </c>
       <c r="E29">
-        <v>69.887120927206908</v>
+        <v>69.88712092720688</v>
       </c>
       <c r="F29">
-        <v>3.6632408000000001</v>
+        <v>2.1880802709178369</v>
       </c>
       <c r="G29">
         <v>3.2055020000000001</v>
       </c>
       <c r="H29">
-        <v>0.46088143534060499</v>
+        <v>0.43040260095465799</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -1228,16 +1204,16 @@
         <v>3</v>
       </c>
       <c r="E30">
-        <v>63.969605931121059</v>
+        <v>63.969605931121009</v>
       </c>
       <c r="F30">
-        <v>3.7106328</v>
+        <v>2.017124564311032</v>
       </c>
       <c r="G30">
         <v>3.1290588000000001</v>
       </c>
       <c r="H30">
-        <v>0.4601000736339671</v>
+        <v>0.42915198416364531</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -1254,16 +1230,16 @@
         <v>3</v>
       </c>
       <c r="E31">
-        <v>62.142828373449447</v>
+        <v>62.142828373449412</v>
       </c>
       <c r="F31">
-        <v>4.8855871999999998</v>
+        <v>3.1507085502191221</v>
       </c>
       <c r="G31">
         <v>4.4643616000000002</v>
       </c>
       <c r="H31">
-        <v>0.47374882819534569</v>
+        <v>0.4509976434605667</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -1280,16 +1256,16 @@
         <v>3</v>
       </c>
       <c r="E32">
-        <v>65.581161113478103</v>
+        <v>65.581161113478089</v>
       </c>
       <c r="F32">
-        <v>5.2054387999999996</v>
+        <v>3.2104471909114061</v>
       </c>
       <c r="G32">
         <v>4.7063192000000003</v>
       </c>
       <c r="H32">
-        <v>0.47622199001052401</v>
+        <v>0.45495608891121719</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -1306,16 +1282,16 @@
         <v>3</v>
       </c>
       <c r="E33">
-        <v>66.503584099270398</v>
+        <v>66.503584099270384</v>
       </c>
       <c r="F33">
-        <v>3.0130756000000001</v>
+        <v>0.99319201384047062</v>
       </c>
       <c r="G33">
         <v>2.5423420000000001</v>
       </c>
       <c r="H33">
-        <v>0.454102966760352</v>
+        <v>0.41955325096501822</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -1332,16 +1308,16 @@
         <v>3</v>
       </c>
       <c r="E34">
-        <v>51.947413505295067</v>
+        <v>51.947413505295103</v>
       </c>
       <c r="F34">
-        <v>2.9860864</v>
+        <v>1.437225846823885</v>
       </c>
       <c r="G34">
         <v>2.5293603999999998</v>
       </c>
       <c r="H34">
-        <v>0.45397027575407689</v>
+        <v>0.41934087096347161</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
@@ -1358,16 +1334,16 @@
         <v>3</v>
       </c>
       <c r="E35">
-        <v>65.765307202688078</v>
+        <v>65.765307202688092</v>
       </c>
       <c r="F35">
-        <v>2.7736855999999999</v>
+        <v>0.54727678879477182</v>
       </c>
       <c r="G35">
         <v>2.3483236000000001</v>
       </c>
       <c r="H35">
-        <v>0.45211981393389822</v>
+        <v>0.41637909461356459</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
@@ -1384,16 +1360,16 @@
         <v>3</v>
       </c>
       <c r="E36">
-        <v>76.224901409392444</v>
+        <v>76.224901409392487</v>
       </c>
       <c r="F36">
-        <v>3.5135412000000001</v>
+        <v>0.71656449351702278</v>
       </c>
       <c r="G36">
         <v>2.9580004</v>
       </c>
       <c r="H36">
-        <v>0.45835160570799388</v>
+        <v>0.42635345522603169</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
@@ -1410,16 +1386,16 @@
         <v>3</v>
       </c>
       <c r="E37">
-        <v>51.071498542238203</v>
+        <v>51.071498542238231</v>
       </c>
       <c r="F37">
-        <v>3.1293712</v>
+        <v>2.0191711733883739</v>
       </c>
       <c r="G37">
         <v>2.6696059999999999</v>
       </c>
       <c r="H37">
-        <v>0.4554037916373006</v>
+        <v>0.42163530005887401</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
@@ -1436,16 +1412,16 @@
         <v>4</v>
       </c>
       <c r="E38">
-        <v>31.03340539157508</v>
+        <v>31.033405391575091</v>
       </c>
       <c r="F38">
-        <v>3.6494569284012002</v>
+        <v>3.649456928401198</v>
       </c>
       <c r="G38">
         <v>2.7353575999999999</v>
       </c>
       <c r="H38">
-        <v>0.7387355048660269</v>
+        <v>0.62714829777093284</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
@@ -1462,16 +1438,16 @@
         <v>4</v>
       </c>
       <c r="E39">
-        <v>40.30246277973032</v>
+        <v>40.302462779730327</v>
       </c>
       <c r="F39">
-        <v>4.1228253723804489</v>
+        <v>4.122825372380448</v>
       </c>
       <c r="G39">
         <v>3.3476656</v>
       </c>
       <c r="H39">
-        <v>0.8720391883430656</v>
+        <v>0.70438359080415669</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
@@ -1488,16 +1464,16 @@
         <v>4</v>
       </c>
       <c r="E40">
-        <v>35.026698768720877</v>
+        <v>35.026698768720863</v>
       </c>
       <c r="F40">
-        <v>4.1585350756274719</v>
+        <v>4.1585350756274764</v>
       </c>
       <c r="G40">
         <v>3.3233923999999999</v>
       </c>
       <c r="H40">
-        <v>0.86675474494239957</v>
+        <v>0.70132181843656749</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
@@ -1514,16 +1490,16 @@
         <v>4</v>
       </c>
       <c r="E41">
-        <v>33.20120752027735</v>
+        <v>33.201207520277343</v>
       </c>
       <c r="F41">
-        <v>4.2457937146676317</v>
+        <v>4.2457937146676326</v>
       </c>
       <c r="G41">
         <v>3.3541968</v>
       </c>
       <c r="H41">
-        <v>0.87346107572249743</v>
+        <v>0.70520742316607077</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
@@ -1540,16 +1516,16 @@
         <v>4</v>
       </c>
       <c r="E42">
-        <v>40.210651591339541</v>
+        <v>40.210651591339563</v>
       </c>
       <c r="F42">
-        <v>4.4521208000000003</v>
+        <v>4.379110136012434</v>
       </c>
       <c r="G42">
         <v>3.7406239999999999</v>
       </c>
       <c r="H42">
-        <v>0.95758894789747817</v>
+        <v>0.75395056881827216</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
@@ -1566,16 +1542,16 @@
         <v>4</v>
       </c>
       <c r="E43">
-        <v>39.39415574301394</v>
+        <v>39.394155743013947</v>
       </c>
       <c r="F43">
-        <v>3.9440324000000002</v>
+        <v>3.5349129922211011</v>
       </c>
       <c r="G43">
         <v>2.9372924</v>
       </c>
       <c r="H43">
-        <v>0.78269810646881366</v>
+        <v>0.65261994513076749</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
@@ -1592,16 +1568,16 @@
         <v>4</v>
       </c>
       <c r="E44">
-        <v>38.633480213372621</v>
+        <v>38.633480213372671</v>
       </c>
       <c r="F44">
-        <v>4.1735787999999996</v>
+        <v>3.9166443275936351</v>
       </c>
       <c r="G44">
         <v>3.2630623999999999</v>
       </c>
       <c r="H44">
-        <v>0.85362048698044291</v>
+        <v>0.69371191422382728</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
@@ -1621,13 +1597,13 @@
         <v>34.934229569144499</v>
       </c>
       <c r="F45">
-        <v>4.9511488000000003</v>
+        <v>4.7834075102524478</v>
       </c>
       <c r="G45">
         <v>3.7892131999999998</v>
       </c>
       <c r="H45">
-        <v>0.96816715255461538</v>
+        <v>0.76007951225890924</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
@@ -1644,16 +1620,16 @@
         <v>4</v>
       </c>
       <c r="E46">
-        <v>29.167243224391878</v>
+        <v>29.1672432243919</v>
       </c>
       <c r="F46">
-        <v>2.8416836000000001</v>
+        <v>2.7297817080074491</v>
       </c>
       <c r="G46">
         <v>2.2022412</v>
       </c>
       <c r="H46">
-        <v>0.62267238003013015</v>
+        <v>0.55990207303629358</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
@@ -1670,7 +1646,7 @@
         <v>4</v>
       </c>
       <c r="E47">
-        <v>30.39107239124121</v>
+        <v>30.39107239124122</v>
       </c>
       <c r="F47">
         <v>2.5579248387752198</v>
@@ -1679,7 +1655,7 @@
         <v>2.0934371999999999</v>
       </c>
       <c r="H47">
-        <v>0.59898499724722409</v>
+        <v>0.54617775647798172</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
@@ -1696,16 +1672,16 @@
         <v>4</v>
       </c>
       <c r="E48">
-        <v>37.514918378828199</v>
+        <v>37.514918378828213</v>
       </c>
       <c r="F48">
-        <v>3.8343379645751692</v>
+        <v>3.8343379645751678</v>
       </c>
       <c r="G48">
         <v>3.1483851999999999</v>
       </c>
       <c r="H48">
-        <v>0.82865446796577569</v>
+        <v>0.67924676409312568</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
@@ -1722,16 +1698,16 @@
         <v>4</v>
       </c>
       <c r="E49">
-        <v>29.536299152482709</v>
+        <v>29.536299152482719</v>
       </c>
       <c r="F49">
-        <v>2.8485229564567351</v>
+        <v>2.8485229564567338</v>
       </c>
       <c r="G49">
         <v>2.2488883999999998</v>
       </c>
       <c r="H49">
-        <v>0.63282779786541932</v>
+        <v>0.56578605652365521</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
@@ -1748,16 +1724,16 @@
         <v>5</v>
       </c>
       <c r="E50">
-        <v>38.260147594924902</v>
+        <v>38.260147594924888</v>
       </c>
       <c r="F50">
-        <v>2.0708468</v>
+        <v>1.8392231365517271</v>
       </c>
       <c r="G50">
         <v>1.640442</v>
       </c>
       <c r="H50">
-        <v>0.36873980424839597</v>
+        <v>0.24365656900995011</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
@@ -1774,16 +1750,16 @@
         <v>5</v>
       </c>
       <c r="E51">
-        <v>55.850517339027618</v>
+        <v>55.850517339027597</v>
       </c>
       <c r="F51">
-        <v>3.1229596000000002</v>
+        <v>2.56592461517242</v>
       </c>
       <c r="G51">
         <v>2.7910751999999999</v>
       </c>
       <c r="H51">
-        <v>0.39276874650181348</v>
+        <v>0.27748573164071999</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
@@ -1800,16 +1776,16 @@
         <v>5</v>
       </c>
       <c r="E52">
-        <v>38.726488446601742</v>
+        <v>38.726488446601728</v>
       </c>
       <c r="F52">
-        <v>3.2545616000000002</v>
+        <v>3.1555439448275808</v>
       </c>
       <c r="G52">
         <v>2.8691928</v>
       </c>
       <c r="H52">
-        <v>0.39440009461463982</v>
+        <v>0.27978242618658022</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
@@ -1829,13 +1805,13 @@
         <v>36.697150666202923</v>
       </c>
       <c r="F53">
-        <v>1.8627836</v>
+        <v>1.7082994289655209</v>
       </c>
       <c r="G53">
         <v>1.5953079999999999</v>
       </c>
       <c r="H53">
-        <v>0.36779726036936838</v>
+        <v>0.24232960797129999</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
@@ -1852,16 +1828,16 @@
         <v>5</v>
       </c>
       <c r="E54">
-        <v>40.246162239179469</v>
+        <v>40.246162239179448</v>
       </c>
       <c r="F54">
-        <v>1.3168184000000001</v>
+        <v>1.110210091034499</v>
       </c>
       <c r="G54">
         <v>1.09985</v>
       </c>
       <c r="H54">
-        <v>0.35745049506571308</v>
+        <v>0.22776290742874991</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
@@ -1878,16 +1854,16 @@
         <v>5</v>
       </c>
       <c r="E55">
-        <v>36.824735693555787</v>
+        <v>36.824735693555802</v>
       </c>
       <c r="F55">
-        <v>2.2943935999999998</v>
+        <v>2.1365562758620702</v>
       </c>
       <c r="G55">
         <v>2.0002032000000001</v>
       </c>
       <c r="H55">
-        <v>0.37625278153761382</v>
+        <v>0.25423371917652032</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
@@ -1904,16 +1880,16 @@
         <v>5</v>
       </c>
       <c r="E56">
-        <v>35.636475586403748</v>
+        <v>35.636475586403762</v>
       </c>
       <c r="F56">
-        <v>2.242945638620689</v>
+        <v>2.2429456386206859</v>
       </c>
       <c r="G56">
         <v>1.8072463999999999</v>
       </c>
       <c r="H56">
-        <v>0.37222321954982812</v>
+        <v>0.24856069760204</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
@@ -1939,7 +1915,7 @@
         <v>1.5735208000000001</v>
       </c>
       <c r="H57">
-        <v>0.36734227317565299</v>
+        <v>0.24168905394238019</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
@@ -1959,13 +1935,13 @@
         <v>32.113745490074983</v>
       </c>
       <c r="F58">
-        <v>1.5008352</v>
+        <v>1.271437313103448</v>
       </c>
       <c r="G58">
         <v>1.1588944000000001</v>
       </c>
       <c r="H58">
-        <v>0.35868353308164003</v>
+        <v>0.22949884083484001</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
@@ -1985,13 +1961,13 @@
         <v>28.61661791928967</v>
       </c>
       <c r="F59">
-        <v>2.6050947999999998</v>
+        <v>2.462465862068965</v>
       </c>
       <c r="G59">
         <v>2.2287835999999999</v>
       </c>
       <c r="H59">
-        <v>0.3810262794967052</v>
+        <v>0.26095409151221022</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
@@ -2008,16 +1984,16 @@
         <v>5</v>
       </c>
       <c r="E60">
-        <v>37.73188563565639</v>
+        <v>37.731885635656383</v>
       </c>
       <c r="F60">
-        <v>1.2863156</v>
+        <v>1.092053227586206</v>
       </c>
       <c r="G60">
         <v>1.0004262399999999</v>
       </c>
       <c r="H60">
-        <v>0.35537420543000858</v>
+        <v>0.22483980165846409</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
@@ -2034,16 +2010,16 @@
         <v>5</v>
       </c>
       <c r="E61">
-        <v>30.618069333361181</v>
+        <v>30.61806933336117</v>
       </c>
       <c r="F61">
-        <v>2.2244655999999998</v>
+        <v>2.0582743448275949</v>
       </c>
       <c r="G61">
         <v>1.8715264</v>
       </c>
       <c r="H61">
-        <v>0.37356559382518317</v>
+        <v>0.25045056013504019</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
@@ -2060,16 +2036,16 @@
         <v>6</v>
       </c>
       <c r="E62">
-        <v>57.674471266819509</v>
+        <v>57.674471266819523</v>
       </c>
       <c r="F62">
-        <v>2.5414843999999999</v>
+        <v>2.3585329183880348</v>
       </c>
       <c r="G62">
         <v>2.0778371999999998</v>
       </c>
       <c r="H62">
-        <v>0.33546763658781492</v>
+        <v>0.23715757524387501</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
@@ -2086,16 +2062,16 @@
         <v>6</v>
       </c>
       <c r="E63">
-        <v>94.480746118664968</v>
+        <v>94.480746118664925</v>
       </c>
       <c r="F63">
-        <v>1.5780335999999999</v>
+        <v>1.473887601191229</v>
       </c>
       <c r="G63">
         <v>1.3897476</v>
       </c>
       <c r="H63">
-        <v>0.229796820907298</v>
+        <v>0.16269529930194859</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
@@ -2112,16 +2088,16 @@
         <v>6</v>
       </c>
       <c r="E64">
-        <v>75.1054740651618</v>
+        <v>75.105474065161843</v>
       </c>
       <c r="F64">
-        <v>1.5060408000000001</v>
+        <v>1.4204650217680299</v>
       </c>
       <c r="G64">
         <v>1.3720920000000001</v>
       </c>
       <c r="H64">
-        <v>0.2270854274298657</v>
+        <v>0.16078468161622819</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
@@ -2138,16 +2114,16 @@
         <v>6</v>
       </c>
       <c r="E65">
-        <v>79.161525431900372</v>
+        <v>79.161525431900344</v>
       </c>
       <c r="F65">
-        <v>4.3660487999999997</v>
+        <v>4.2084359484040386</v>
       </c>
       <c r="G65">
         <v>3.8607551999999998</v>
       </c>
       <c r="H65">
-        <v>0.60927267498902893</v>
+        <v>0.4300977564322368</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
@@ -2164,16 +2140,16 @@
         <v>6</v>
       </c>
       <c r="E66">
-        <v>67.854038861470499</v>
+        <v>67.854038861470556</v>
       </c>
       <c r="F66">
-        <v>2.8131864000000002</v>
+        <v>2.6275578192598559</v>
       </c>
       <c r="G66">
         <v>2.3227440000000001</v>
       </c>
       <c r="H66">
-        <v>0.37307829270252052</v>
+        <v>0.26366039947149611</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
@@ -2190,16 +2166,16 @@
         <v>6</v>
       </c>
       <c r="E67">
-        <v>64.906499630975745</v>
+        <v>64.906499630975759</v>
       </c>
       <c r="F67">
-        <v>2.9812976</v>
+        <v>2.785727588614205</v>
       </c>
       <c r="G67">
         <v>2.5866435999999999</v>
       </c>
       <c r="H67">
-        <v>0.41360569783952877</v>
+        <v>0.29221854776521239</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
@@ -2216,16 +2192,16 @@
         <v>6</v>
       </c>
       <c r="E68">
-        <v>73.709617252419378</v>
+        <v>73.709617252419449</v>
       </c>
       <c r="F68">
-        <v>3.5990172</v>
+        <v>3.3901926138951519</v>
       </c>
       <c r="G68">
         <v>3.084622</v>
       </c>
       <c r="H68">
-        <v>0.49008088903451069</v>
+        <v>0.34610775788249798</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
@@ -2242,16 +2218,16 @@
         <v>6</v>
       </c>
       <c r="E69">
-        <v>57.514599897060073</v>
+        <v>57.514599897060123</v>
       </c>
       <c r="F69">
-        <v>2.1695136000000002</v>
+        <v>2.032602994309427</v>
       </c>
       <c r="G69">
         <v>1.8324768</v>
       </c>
       <c r="H69">
-        <v>0.29778732053057771</v>
+        <v>0.21060566425725111</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
@@ -2268,16 +2244,16 @@
         <v>6</v>
       </c>
       <c r="E70">
-        <v>53.484773723160913</v>
+        <v>53.484773723160899</v>
       </c>
       <c r="F70">
-        <v>1.5131364</v>
+        <v>1.4237682662099369</v>
       </c>
       <c r="G70">
         <v>1.3272796</v>
       </c>
       <c r="H70">
-        <v>0.22020352882160091</v>
+        <v>0.15593526477513639</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
@@ -2294,16 +2270,16 @@
         <v>6</v>
       </c>
       <c r="E71">
-        <v>57.298908353829653</v>
+        <v>57.29890835382966</v>
       </c>
       <c r="F71">
-        <v>1.4594516</v>
+        <v>1.351611032461939</v>
       </c>
       <c r="G71">
         <v>1.2634955999999999</v>
       </c>
       <c r="H71">
-        <v>0.21040813690263269</v>
+        <v>0.14903281804628049</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
@@ -2323,13 +2299,13 @@
         <v>68.251183877571108</v>
       </c>
       <c r="F72">
-        <v>2.6101535999999999</v>
+        <v>2.4576281941402049</v>
       </c>
       <c r="G72">
         <v>2.2305624000000002</v>
       </c>
       <c r="H72">
-        <v>0.35892184438134928</v>
+        <v>0.25368487922534172</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
@@ -2346,20 +2322,19 @@
         <v>6</v>
       </c>
       <c r="E73">
-        <v>58.956904743376683</v>
+        <v>58.956904743376697</v>
       </c>
       <c r="F73">
-        <v>1.5795448000000001</v>
+        <v>1.4779031796580671</v>
       </c>
       <c r="G73">
         <v>1.3753576000000001</v>
       </c>
       <c r="H73">
-        <v>0.2275869298732778</v>
+        <v>0.16113807165193861</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H73" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>